<commit_message>
Updated tracker -- vipin
</commit_message>
<xml_diff>
--- a/Docs/Tasks_Tracker.xlsx
+++ b/Docs/Tasks_Tracker.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$43</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="72">
   <si>
     <t>S.No.</t>
   </si>
@@ -223,6 +223,18 @@
   </si>
   <si>
     <t>Need testing</t>
+  </si>
+  <si>
+    <t>Add Visitor Manually</t>
+  </si>
+  <si>
+    <t>Visitor by scan image</t>
+  </si>
+  <si>
+    <t>Visitor List</t>
+  </si>
+  <si>
+    <t>Visitor</t>
   </si>
 </sst>
 </file>
@@ -571,9 +583,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -639,7 +654,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -696,7 +711,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" hidden="1">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -717,7 +732,7 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" hidden="1">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -754,7 +769,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="30">
+    <row r="9" spans="1:7" ht="30" hidden="1">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -794,7 +809,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30">
+    <row r="11" spans="1:7" ht="30" hidden="1">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -814,7 +829,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30">
+    <row r="12" spans="1:7" ht="30" hidden="1">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -854,7 +869,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30">
+    <row r="14" spans="1:7" ht="30" hidden="1">
       <c r="A14" s="2">
         <v>14</v>
       </c>
@@ -872,7 +887,7 @@
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:7" ht="30">
+    <row r="15" spans="1:7" ht="30" hidden="1">
       <c r="A15" s="2">
         <v>15</v>
       </c>
@@ -888,7 +903,7 @@
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" hidden="1">
       <c r="A16" s="2">
         <v>16</v>
       </c>
@@ -906,7 +921,7 @@
       </c>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" hidden="1">
       <c r="A17" s="2">
         <v>17</v>
       </c>
@@ -924,7 +939,7 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" hidden="1">
       <c r="A18" s="2">
         <v>18</v>
       </c>
@@ -960,7 +975,7 @@
       </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:7" ht="30">
+    <row r="20" spans="1:7" ht="30" hidden="1">
       <c r="A20" s="2">
         <v>20</v>
       </c>
@@ -978,7 +993,7 @@
       </c>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" hidden="1">
       <c r="A21" s="2">
         <v>21</v>
       </c>
@@ -996,7 +1011,7 @@
       </c>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" hidden="1">
       <c r="A22" s="2">
         <v>22</v>
       </c>
@@ -1017,7 +1032,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" hidden="1">
       <c r="A23" s="2">
         <v>23</v>
       </c>
@@ -1037,7 +1052,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30">
+    <row r="24" spans="1:7" ht="30" hidden="1">
       <c r="A24" s="2">
         <v>24</v>
       </c>
@@ -1077,7 +1092,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" hidden="1">
       <c r="A26" s="2">
         <v>26</v>
       </c>
@@ -1094,7 +1109,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" hidden="1">
       <c r="A27" s="2">
         <v>27</v>
       </c>
@@ -1111,7 +1126,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" hidden="1">
       <c r="A28" s="2">
         <v>28</v>
       </c>
@@ -1128,7 +1143,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" hidden="1">
       <c r="A29" s="2">
         <v>29</v>
       </c>
@@ -1145,7 +1160,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" hidden="1">
       <c r="A30" s="2">
         <v>30</v>
       </c>
@@ -1162,7 +1177,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" hidden="1">
       <c r="A31" s="2">
         <v>31</v>
       </c>
@@ -1179,7 +1194,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" hidden="1">
       <c r="A32" s="2">
         <v>32</v>
       </c>
@@ -1196,7 +1211,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" hidden="1">
       <c r="A33" s="2">
         <v>33</v>
       </c>
@@ -1234,7 +1249,7 @@
       </c>
       <c r="G34" s="2"/>
     </row>
-    <row r="35" spans="1:7" ht="30">
+    <row r="35" spans="1:7" ht="30" hidden="1">
       <c r="A35" s="2">
         <v>24</v>
       </c>
@@ -1251,7 +1266,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" hidden="1">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1268,7 +1283,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" hidden="1">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1302,7 +1317,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" hidden="1">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1319,7 +1334,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" hidden="1">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1337,25 +1352,55 @@
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="44" spans="1:7">
       <c r="A44" s="2"/>
@@ -1708,8 +1753,12 @@
       <c r="E93" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G40">
-    <filterColumn colId="2"/>
+  <autoFilter ref="A1:G43">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Shambhoo"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="4"/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>